<commit_message>
Add Validacion de Fecha
Se adiciona validacion de la existencia del campo de fecha
</commit_message>
<xml_diff>
--- a/sourceORCID/source_orcid.xlsx
+++ b/sourceORCID/source_orcid.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kimba\Documents\Kimping\Personal\ServicioSocial\Pruebas\API_Consumo\sourceORCID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kimba\Documents\Kimping\Personal\ServicioSocial\Pruebas\Python_ORCID\sourceORCID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D59A6A-2A10-4FB2-91A2-A59CCC018039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1E1471-2FAB-49BA-9914-DA29A9694439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{629CD8D1-CFBD-49D3-A343-23419FFB5836}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>0000-0003-4473-4471</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>xxxxxx</t>
+  </si>
+  <si>
+    <t>0000-0001-9578-9064</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEDD69B-7333-4EA0-A1A0-83395DC5D7C2}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +473,7 @@
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -478,47 +481,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E7" s="2"/>
     </row>
   </sheetData>

</xml_diff>